<commit_message>
changing sceript for selection of param
</commit_message>
<xml_diff>
--- a/RevisionSequence/Inventory.xlsx
+++ b/RevisionSequence/Inventory.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/leahbriscoe/Documents/MicroBatch/microbatch_vc/RevisionSequence/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{ABFD1735-9D4B-F44A-9306-CADFE86428E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A90A5577-47AB-0C4F-9518-27FC5EA61AAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1500" windowWidth="28040" windowHeight="17440" xr2:uid="{71B07BF1-56F0-F64A-8E8F-42CF3E570058}"/>
+    <workbookView xWindow="-30660" yWindow="1420" windowWidth="28040" windowHeight="17440" xr2:uid="{71B07BF1-56F0-F64A-8E8F-42CF3E570058}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="RF" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,6 +32,53 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="14">
+  <si>
+    <t>Gibbonsr_complete_otu</t>
+  </si>
+  <si>
+    <t>AGPr_complete_otu</t>
+  </si>
+  <si>
+    <t>Thomasr_complete_otu</t>
+  </si>
+  <si>
+    <t>AGPr_max_k5</t>
+  </si>
+  <si>
+    <t>AGPr_max_k6</t>
+  </si>
+  <si>
+    <t>AGPr_max_k7</t>
+  </si>
+  <si>
+    <t>uncorrected</t>
+  </si>
+  <si>
+    <t>bmc</t>
+  </si>
+  <si>
+    <t>combat</t>
+  </si>
+  <si>
+    <t>limma</t>
+  </si>
+  <si>
+    <t>DCC</t>
+  </si>
+  <si>
+    <t>clr_pcacounts</t>
+  </si>
+  <si>
+    <t>clr_pca1</t>
+  </si>
+  <si>
+    <t>clr_pcaroundcounts</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -380,9 +428,156 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADAD7830-0091-B848-B9AF-998645F659F2}">
+  <dimension ref="A1:R8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L9" sqref="L9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.83203125" customWidth="1"/>
+    <col min="7" max="9" width="16.83203125" customWidth="1"/>
+    <col min="11" max="11" width="15.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="G1">
+        <v>1</v>
+      </c>
+      <c r="H1">
+        <v>1</v>
+      </c>
+      <c r="I1">
+        <v>1</v>
+      </c>
+      <c r="J1">
+        <v>2</v>
+      </c>
+      <c r="K1">
+        <v>2</v>
+      </c>
+      <c r="L1">
+        <v>2</v>
+      </c>
+      <c r="M1">
+        <v>3</v>
+      </c>
+      <c r="N1">
+        <v>3</v>
+      </c>
+      <c r="O1">
+        <v>3</v>
+      </c>
+      <c r="P1">
+        <v>4</v>
+      </c>
+      <c r="Q1">
+        <v>4</v>
+      </c>
+      <c r="R1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" t="s">
+        <v>13</v>
+      </c>
+      <c r="J2" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" t="s">
+        <v>11</v>
+      </c>
+      <c r="L2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" t="s">
+        <v>12</v>
+      </c>
+      <c r="N2" t="s">
+        <v>11</v>
+      </c>
+      <c r="O2" t="s">
+        <v>13</v>
+      </c>
+      <c r="P2" t="s">
+        <v>12</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>11</v>
+      </c>
+      <c r="R2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="J4">
+        <v>27</v>
+      </c>
+      <c r="L4">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A940F727-A841-7A4A-B605-E6F249B58C74}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData/>

</xml_diff>